<commit_message>
REGARDER TEST UNIT MOCHA
https://mochajs.org
</commit_message>
<xml_diff>
--- a/DOC AFPA J Jacques/Planning_Pense-Bete.xlsx
+++ b/DOC AFPA J Jacques/Planning_Pense-Bete.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\titi\Documents\persoNotes\DOC AFPA J Jacques\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="60" windowWidth="9300" windowHeight="4080"/>
+    <workbookView xWindow="1335" yWindow="60" windowWidth="9300" windowHeight="4080"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -172,9 +177,6 @@
     <t>* Documenter au fur et à mesure</t>
   </si>
   <si>
-    <t>* Avancer le rapport de stage au fur et à mesure</t>
-  </si>
-  <si>
     <t>* Découper le projet en petits sprints (Méthode agile)</t>
   </si>
   <si>
@@ -264,13 +266,16 @@
   </si>
   <si>
     <t>* Faire un tableur des fonctionnalités avec une colonne satisfaction</t>
+  </si>
+  <si>
+    <t>faire des test unitaires en java script</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,12 +308,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -483,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,9 +516,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -520,25 +534,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,6 +570,14 @@
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -596,7 +624,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,9 +656,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -662,6 +691,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -837,650 +867,650 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" customWidth="1"/>
-    <col min="3" max="3" width="86.54296875" customWidth="1"/>
-    <col min="4" max="4" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="86.5703125" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="37.5" thickBot="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17" t="s">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>2</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="B12" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="11"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="11"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
-      <c r="A12" s="11">
-        <v>2</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="11"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17" t="s">
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="11"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17" t="s">
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="11"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="11"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="11"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="str">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="str">
         <f>"           =&gt; et appeler ses fonctions nom_main_function.ma_function()"</f>
         <v xml:space="preserve">           =&gt; et appeler ses fonctions nom_main_function.ma_function()</v>
       </c>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="27" t="s">
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="11"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="14"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="11"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17" t="s">
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="11"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17" t="s">
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="11"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17" t="s">
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17" t="s">
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="11"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17" t="s">
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="11"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17" t="s">
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="14"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="27" t="s">
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="11"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17" t="s">
+      <c r="C30" s="26"/>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="11"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17" t="s">
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="14"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="11"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17" t="s">
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17" t="s">
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
+        <v>3</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="11"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="14"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="14"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1">
-      <c r="A37" s="11">
-        <v>3</v>
-      </c>
-      <c r="B37" s="27" t="s">
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="13"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="11"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="14"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="11"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="14"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="11"/>
-      <c r="B41" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="14"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="11"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1">
-      <c r="A43" s="11"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="14" t="s">
+      <c r="C44" s="23"/>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="11"/>
-      <c r="B44" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="14"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="11"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="14" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="11"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="14" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="11"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="14" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="11"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D48" s="14" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="13"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10">
+        <v>8</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="24"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="13"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="13"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="13"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="10"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="13"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="11"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="14"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="11"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D50" s="14"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1">
-      <c r="A51" s="11"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="14"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1">
-      <c r="A52" s="11">
-        <v>8</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="14"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="11"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="11"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="14"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="11"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D55" s="14"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="11"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="14"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="11"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D57" s="14"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="11"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="14"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1">
-      <c r="A59" s="11"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="14"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1">
-      <c r="A60" s="11"/>
-      <c r="B60" s="27" t="s">
+      <c r="C60" s="26"/>
+      <c r="D60" s="13"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="28"/>
-      <c r="D60" s="14"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="11"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="17" t="s">
+      <c r="D61" s="13"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="14"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="11"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17" t="s">
+      <c r="D62" s="13"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="14"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="11"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63" s="14"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1">
-      <c r="A64" s="11"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="14"/>
-    </row>
-    <row r="65" spans="1:4" ht="15" thickBot="1">
-      <c r="A65" s="11">
+      <c r="D63" s="13"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="13"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10">
         <v>9</v>
       </c>
-      <c r="B65" s="27" t="s">
+      <c r="B65" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="28"/>
-      <c r="D65" s="14"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="11"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="13"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
       <c r="B66" s="5"/>
       <c r="C66" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="14"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="11"/>
+      <c r="D66" s="13"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
       <c r="B67" s="5"/>
       <c r="C67" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="14"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="11"/>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
       <c r="B68" s="5"/>
       <c r="C68" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="14"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="11"/>
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
       <c r="B69" s="5"/>
       <c r="C69" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="14"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="11"/>
+      <c r="D69" s="13"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
       <c r="B70" s="5"/>
       <c r="C70" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D70" s="14"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="11"/>
+      <c r="D70" s="13"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
       <c r="B71" s="5"/>
       <c r="C71" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D71" s="14"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="11"/>
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
       <c r="B72" s="5"/>
       <c r="C72" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D72" s="14"/>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="11"/>
+      <c r="D72" s="13"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
       <c r="B73" s="5"/>
       <c r="C73" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D73" s="14"/>
-    </row>
-    <row r="74" spans="1:4" ht="15" thickBot="1">
-      <c r="A74" s="12"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="15"/>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="11"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1501,24 +1531,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>